<commit_message>
Update Sensitivity Analysis of Marketing Strategies.xlsx
</commit_message>
<xml_diff>
--- a/Sensitivity Analysis of Marketing Strategies.xlsx
+++ b/Sensitivity Analysis of Marketing Strategies.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/madittmer_2018_socsc_smu_edu_sg/Documents/University Stuff/Year 2 Sem 2/4. Spreadsheet Modeling &amp; Analytics/Project/SMA-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LIYAO\OneDrive - Singapore Management University\SMA G7\Group Project\Github\SMA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2D29F41-F614-40AF-8A5B-C4456C386DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92560B06-798D-4FC3-9F0B-9FF2B63F9308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{47D6FB81-707F-442F-B7B5-908A315AAEB2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{47D6FB81-707F-442F-B7B5-908A315AAEB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Social Media" sheetId="1" r:id="rId1"/>
-    <sheet name="Fave" sheetId="4" r:id="rId2"/>
+    <sheet name="SEO" sheetId="4" r:id="rId2"/>
     <sheet name="Google " sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t xml:space="preserve">Revenue </t>
   </si>
@@ -59,9 +59,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -162,7 +163,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -190,6 +191,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1696,6 +1700,1453 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-SG"/>
+              <a:t>Sensitivity</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-SG" baseline="0"/>
+              <a:t> Analysis of SEO</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-SG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>136.26899999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.43199999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140.595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142.75800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144.92100000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147.084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>149.24700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151.41000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>153.57299999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>155.73599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>157.899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160.06199999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>162.22499999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>164.38800000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>166.55100000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>168.714</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170.87699999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>149.89589999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.27520000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.65449999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>157.03380000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>159.41310000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>161.79240000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>164.17170000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>166.55100000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168.93029999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>171.30959999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>173.68889999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176.06819999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178.44749999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>180.82679999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>183.20609999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>185.58539999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>187.96469999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$8:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>163.52279999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166.11839999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168.71400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>171.30960000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173.90520000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.5008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>179.09640000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>181.69200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184.2876</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>186.88319999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>189.47879999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>192.07439999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>194.67</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>197.26560000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>199.8612</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>202.45679999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>205.05240000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$9:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>177.1497</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>179.9616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>182.77350000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.58540000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.39730000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>191.20920000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>194.02110000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>196.83300000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199.64489999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>202.45679999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>205.2687</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>208.0806</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210.89250000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>213.70439999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>216.5163</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>219.32820000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>222.14009999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$10:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>190.7766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193.8048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.833</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199.86120000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>202.88939999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>205.91760000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>208.94580000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211.97400000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>215.00219999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>218.03039999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>221.05859999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>224.08679999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>227.11500000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230.14319999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>233.17139999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>236.19959999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>239.2278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$11:$S$11</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>204.40350000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210.89250000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>214.13700000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>217.38150000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>220.626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>223.87050000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>227.11500000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230.35949999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>233.60399999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>236.8485</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240.09299999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>243.33750000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>246.58199999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>249.82649999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>253.071</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>256.31549999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$12:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>218.03040000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>221.49119999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>224.95200000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>228.4128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231.87360000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>235.33440000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>238.79520000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>242.256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>245.71679999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>249.17759999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>252.63839999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256.0992</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>259.56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>263.02079999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>266.48160000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>269.94239999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>273.40320000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$13:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>231.65730000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>235.33440000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>239.01149999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.68860000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>246.3657</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250.0428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>253.71990000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>257.39699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>261.07409999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>264.75119999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>268.42829999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>272.10539999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>275.78249999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>279.45959999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>283.13669999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>286.81380000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>290.49090000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>245.28420000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>249.17760000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253.071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256.96440000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260.8578</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264.75120000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>268.64460000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>272.53800000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>276.4314</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280.32479999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>284.21819999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>288.11160000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>292.005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>295.89839999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>299.79179999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>303.68519999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>307.57860000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$15:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>258.91110000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>263.02080000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>267.13050000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>271.24020000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>275.34990000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>279.45960000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>283.56930000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>287.67900000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>291.78870000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>295.89839999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300.00810000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>304.11779999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>308.22750000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312.3372</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>316.44690000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>320.5566</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>324.66629999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$16:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>272.53799999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>276.86399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>281.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>285.51600000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>289.84200000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294.16800000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>298.49400000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302.82000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>307.14599999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>311.47199999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>315.798</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>320.12399999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>324.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>328.77600000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>333.10200000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>337.428</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>341.75399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$17:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>286.16489999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>290.7072</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>295.24950000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>299.79180000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>304.33409999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>308.87640000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>313.41870000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>317.96100000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>322.50329999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>327.04559999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>331.58789999999993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>336.1302</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>340.67250000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>345.21479999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>349.75709999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>354.29939999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>358.8417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$18:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>299.79179999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>304.55040000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>309.30899999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>314.06760000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>318.82620000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>323.58480000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>328.34340000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>333.10200000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>337.86059999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>342.61919999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>347.37779999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>352.13639999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>356.89499999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>361.65359999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>366.41219999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>371.17079999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>375.92939999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SEO!$C$19:$S$19</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>313.4187</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>318.39360000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>323.36849999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>328.34339999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>333.31830000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>338.29320000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>343.26810000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>348.24300000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>353.21789999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>358.19279999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>363.16769999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>368.14259999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>373.11750000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378.0924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>383.06729999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>388.04219999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>393.01709999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-A11D-4168-89C3-659F346699FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="763818776"/>
+        <c:axId val="763816808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="763818776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763816808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="763816808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763818776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
               <a:t>Sensitivity Analysis of Google My Business</a:t>
             </a:r>
           </a:p>
@@ -1765,7 +3216,7 @@
             <c:numRef>
               <c:f>'Google '!$C$6:$S$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>35.559000000000005</c:v>
@@ -1847,7 +3298,7 @@
             <c:numRef>
               <c:f>'Google '!$C$7:$S$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>36.876000000000005</c:v>
@@ -1929,7 +3380,7 @@
             <c:numRef>
               <c:f>'Google '!$C$8:$S$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>38.192999999999998</c:v>
@@ -2011,7 +3462,7 @@
             <c:numRef>
               <c:f>'Google '!$C$9:$S$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>39.51</c:v>
@@ -2093,7 +3544,7 @@
             <c:numRef>
               <c:f>'Google '!$C$10:$S$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>40.826999999999998</c:v>
@@ -2175,7 +3626,7 @@
             <c:numRef>
               <c:f>'Google '!$C$11:$S$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>42.144000000000005</c:v>
@@ -2259,7 +3710,7 @@
             <c:numRef>
               <c:f>'Google '!$C$12:$S$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>43.461000000000006</c:v>
@@ -2343,7 +3794,7 @@
             <c:numRef>
               <c:f>'Google '!$C$13:$S$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>44.777999999999999</c:v>
@@ -2427,7 +3878,7 @@
             <c:numRef>
               <c:f>'Google '!$C$14:$S$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>46.094999999999999</c:v>
@@ -2511,7 +3962,7 @@
             <c:numRef>
               <c:f>'Google '!$C$15:$S$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>47.411999999999999</c:v>
@@ -2595,7 +4046,7 @@
             <c:numRef>
               <c:f>'Google '!$C$16:$S$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>48.728999999999999</c:v>
@@ -2679,7 +4130,7 @@
             <c:numRef>
               <c:f>'Google '!$C$17:$S$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>50.046000000000006</c:v>
@@ -2764,7 +4215,7 @@
             <c:numRef>
               <c:f>'Google '!$C$18:$S$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>51.363</c:v>
@@ -2849,7 +4300,7 @@
             <c:numRef>
               <c:f>'Google '!$C$19:$S$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>52.68</c:v>
@@ -2995,7 +4446,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3154,6 +4605,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4225,6 +5716,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4267,6 +6274,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2835C913-7507-49A0-BD8D-90D97423630F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4606,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C3465F-F7FA-4C05-9779-9F86EE094B58}">
   <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="69" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5532,15 +7580,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE27D5C6-A73D-453B-8970-5BEBA7CFED28}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:19" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5550,182 +7598,895 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D3" s="11">
+        <f>(G3+H3)/2</f>
+        <v>3.605</v>
+      </c>
+      <c r="E3" s="18">
+        <f>PRODUCT(B3:D3)</f>
+        <v>52.632999999999996</v>
+      </c>
+      <c r="F3" s="12">
+        <v>5.96</v>
+      </c>
+      <c r="G3" s="12">
+        <v>7.21</v>
+      </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B5" s="8">
+        <f>E3</f>
+        <v>52.632999999999996</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.126</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.128</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="I5" s="20">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J5" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L5" s="20">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="M5" s="20">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="N5" s="20">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="P5" s="20">
+        <v>0.152</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>0.154</v>
+      </c>
+      <c r="R5" s="20">
+        <v>0.156</v>
+      </c>
+      <c r="S5" s="20">
+        <v>0.158</v>
+      </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B6" s="2">
+        <v>300</v>
+      </c>
+      <c r="C6" s="21">
+        <f t="dataTable" ref="C6:S19" dt2D="1" dtr="1" r1="C3" r2="B3"/>
+        <v>136.26899999999998</v>
+      </c>
+      <c r="D6" s="21">
+        <v>138.43199999999999</v>
+      </c>
+      <c r="E6" s="21">
+        <v>140.595</v>
+      </c>
+      <c r="F6" s="21">
+        <v>142.75800000000001</v>
+      </c>
+      <c r="G6" s="21">
+        <v>144.92100000000002</v>
+      </c>
+      <c r="H6" s="21">
+        <v>147.084</v>
+      </c>
+      <c r="I6" s="21">
+        <v>149.24700000000001</v>
+      </c>
+      <c r="J6" s="21">
+        <v>151.41000000000003</v>
+      </c>
+      <c r="K6" s="21">
+        <v>153.57299999999998</v>
+      </c>
+      <c r="L6" s="21">
+        <v>155.73599999999999</v>
+      </c>
+      <c r="M6" s="21">
+        <v>157.899</v>
+      </c>
+      <c r="N6" s="21">
+        <v>160.06199999999998</v>
+      </c>
+      <c r="O6" s="21">
+        <v>162.22499999999999</v>
+      </c>
+      <c r="P6" s="21">
+        <v>164.38800000000001</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>166.55100000000002</v>
+      </c>
+      <c r="R6" s="21">
+        <v>168.714</v>
+      </c>
+      <c r="S6" s="21">
+        <v>170.87699999999998</v>
+      </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="2">
+        <v>330</v>
+      </c>
+      <c r="C7" s="21">
+        <v>149.89589999999998</v>
+      </c>
+      <c r="D7" s="21">
+        <v>152.27520000000001</v>
+      </c>
+      <c r="E7" s="21">
+        <v>154.65449999999998</v>
+      </c>
+      <c r="F7" s="21">
+        <v>157.03380000000001</v>
+      </c>
+      <c r="G7" s="21">
+        <v>159.41310000000001</v>
+      </c>
+      <c r="H7" s="21">
+        <v>161.79240000000001</v>
+      </c>
+      <c r="I7" s="21">
+        <v>164.17170000000002</v>
+      </c>
+      <c r="J7" s="21">
+        <v>166.55100000000002</v>
+      </c>
+      <c r="K7" s="21">
+        <v>168.93029999999996</v>
+      </c>
+      <c r="L7" s="21">
+        <v>171.30959999999999</v>
+      </c>
+      <c r="M7" s="21">
+        <v>173.68889999999999</v>
+      </c>
+      <c r="N7" s="21">
+        <v>176.06819999999999</v>
+      </c>
+      <c r="O7" s="21">
+        <v>178.44749999999999</v>
+      </c>
+      <c r="P7" s="21">
+        <v>180.82679999999999</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>183.20609999999999</v>
+      </c>
+      <c r="R7" s="21">
+        <v>185.58539999999999</v>
+      </c>
+      <c r="S7" s="21">
+        <v>187.96469999999999</v>
+      </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
+        <v>360</v>
+      </c>
+      <c r="C8" s="21">
+        <v>163.52279999999999</v>
+      </c>
+      <c r="D8" s="21">
+        <v>166.11839999999998</v>
+      </c>
+      <c r="E8" s="21">
+        <v>168.71400000000003</v>
+      </c>
+      <c r="F8" s="21">
+        <v>171.30960000000002</v>
+      </c>
+      <c r="G8" s="21">
+        <v>173.90520000000001</v>
+      </c>
+      <c r="H8" s="21">
+        <v>176.5008</v>
+      </c>
+      <c r="I8" s="21">
+        <v>179.09640000000002</v>
+      </c>
+      <c r="J8" s="21">
+        <v>181.69200000000001</v>
+      </c>
+      <c r="K8" s="21">
+        <v>184.2876</v>
+      </c>
+      <c r="L8" s="21">
+        <v>186.88319999999999</v>
+      </c>
+      <c r="M8" s="21">
+        <v>189.47879999999998</v>
+      </c>
+      <c r="N8" s="21">
+        <v>192.07439999999997</v>
+      </c>
+      <c r="O8" s="21">
+        <v>194.67</v>
+      </c>
+      <c r="P8" s="21">
+        <v>197.26560000000001</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>199.8612</v>
+      </c>
+      <c r="R8" s="21">
+        <v>202.45679999999999</v>
+      </c>
+      <c r="S8" s="21">
+        <v>205.05240000000001</v>
+      </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B9" s="2">
+        <v>390</v>
+      </c>
+      <c r="C9" s="21">
+        <v>177.1497</v>
+      </c>
+      <c r="D9" s="21">
+        <v>179.9616</v>
+      </c>
+      <c r="E9" s="21">
+        <v>182.77350000000001</v>
+      </c>
+      <c r="F9" s="21">
+        <v>185.58540000000002</v>
+      </c>
+      <c r="G9" s="21">
+        <v>188.39730000000003</v>
+      </c>
+      <c r="H9" s="21">
+        <v>191.20920000000001</v>
+      </c>
+      <c r="I9" s="21">
+        <v>194.02110000000002</v>
+      </c>
+      <c r="J9" s="21">
+        <v>196.83300000000003</v>
+      </c>
+      <c r="K9" s="21">
+        <v>199.64489999999998</v>
+      </c>
+      <c r="L9" s="21">
+        <v>202.45679999999999</v>
+      </c>
+      <c r="M9" s="21">
+        <v>205.2687</v>
+      </c>
+      <c r="N9" s="21">
+        <v>208.0806</v>
+      </c>
+      <c r="O9" s="21">
+        <v>210.89250000000001</v>
+      </c>
+      <c r="P9" s="21">
+        <v>213.70439999999999</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>216.5163</v>
+      </c>
+      <c r="R9" s="21">
+        <v>219.32820000000001</v>
+      </c>
+      <c r="S9" s="21">
+        <v>222.14009999999999</v>
+      </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>420</v>
+      </c>
+      <c r="C10" s="21">
+        <v>190.7766</v>
+      </c>
+      <c r="D10" s="21">
+        <v>193.8048</v>
+      </c>
+      <c r="E10" s="21">
+        <v>196.833</v>
+      </c>
+      <c r="F10" s="21">
+        <v>199.86120000000003</v>
+      </c>
+      <c r="G10" s="21">
+        <v>202.88939999999999</v>
+      </c>
+      <c r="H10" s="21">
+        <v>205.91760000000002</v>
+      </c>
+      <c r="I10" s="21">
+        <v>208.94580000000002</v>
+      </c>
+      <c r="J10" s="21">
+        <v>211.97400000000002</v>
+      </c>
+      <c r="K10" s="21">
+        <v>215.00219999999999</v>
+      </c>
+      <c r="L10" s="21">
+        <v>218.03039999999999</v>
+      </c>
+      <c r="M10" s="21">
+        <v>221.05859999999998</v>
+      </c>
+      <c r="N10" s="21">
+        <v>224.08679999999998</v>
+      </c>
+      <c r="O10" s="21">
+        <v>227.11500000000001</v>
+      </c>
+      <c r="P10" s="21">
+        <v>230.14319999999998</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>233.17139999999998</v>
+      </c>
+      <c r="R10" s="21">
+        <v>236.19959999999998</v>
+      </c>
+      <c r="S10" s="21">
+        <v>239.2278</v>
+      </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
+        <v>450</v>
+      </c>
+      <c r="C11" s="21">
+        <v>204.40350000000001</v>
+      </c>
+      <c r="D11" s="21">
+        <v>207.648</v>
+      </c>
+      <c r="E11" s="21">
+        <v>210.89250000000001</v>
+      </c>
+      <c r="F11" s="21">
+        <v>214.13700000000003</v>
+      </c>
+      <c r="G11" s="21">
+        <v>217.38150000000002</v>
+      </c>
+      <c r="H11" s="21">
+        <v>220.626</v>
+      </c>
+      <c r="I11" s="21">
+        <v>223.87050000000002</v>
+      </c>
+      <c r="J11" s="21">
+        <v>227.11500000000004</v>
+      </c>
+      <c r="K11" s="21">
+        <v>230.35949999999997</v>
+      </c>
+      <c r="L11" s="21">
+        <v>233.60399999999998</v>
+      </c>
+      <c r="M11" s="21">
+        <v>236.8485</v>
+      </c>
+      <c r="N11" s="21">
+        <v>240.09299999999999</v>
+      </c>
+      <c r="O11" s="21">
+        <v>243.33750000000001</v>
+      </c>
+      <c r="P11" s="21">
+        <v>246.58199999999997</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>249.82649999999998</v>
+      </c>
+      <c r="R11" s="21">
+        <v>253.071</v>
+      </c>
+      <c r="S11" s="21">
+        <v>256.31549999999999</v>
+      </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
+        <v>480</v>
+      </c>
+      <c r="C12" s="21">
+        <v>218.03040000000001</v>
+      </c>
+      <c r="D12" s="21">
+        <v>221.49119999999999</v>
+      </c>
+      <c r="E12" s="21">
+        <v>224.95200000000003</v>
+      </c>
+      <c r="F12" s="21">
+        <v>228.4128</v>
+      </c>
+      <c r="G12" s="21">
+        <v>231.87360000000004</v>
+      </c>
+      <c r="H12" s="21">
+        <v>235.33440000000002</v>
+      </c>
+      <c r="I12" s="21">
+        <v>238.79520000000002</v>
+      </c>
+      <c r="J12" s="21">
+        <v>242.256</v>
+      </c>
+      <c r="K12" s="21">
+        <v>245.71679999999998</v>
+      </c>
+      <c r="L12" s="21">
+        <v>249.17759999999996</v>
+      </c>
+      <c r="M12" s="21">
+        <v>252.63839999999999</v>
+      </c>
+      <c r="N12" s="21">
+        <v>256.0992</v>
+      </c>
+      <c r="O12" s="21">
+        <v>259.56</v>
+      </c>
+      <c r="P12" s="21">
+        <v>263.02079999999995</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>266.48160000000001</v>
+      </c>
+      <c r="R12" s="21">
+        <v>269.94239999999996</v>
+      </c>
+      <c r="S12" s="21">
+        <v>273.40320000000003</v>
+      </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B13" s="2">
+        <v>510</v>
+      </c>
+      <c r="C13" s="21">
+        <v>231.65730000000002</v>
+      </c>
+      <c r="D13" s="21">
+        <v>235.33440000000002</v>
+      </c>
+      <c r="E13" s="21">
+        <v>239.01149999999998</v>
+      </c>
+      <c r="F13" s="21">
+        <v>242.68860000000004</v>
+      </c>
+      <c r="G13" s="21">
+        <v>246.3657</v>
+      </c>
+      <c r="H13" s="21">
+        <v>250.0428</v>
+      </c>
+      <c r="I13" s="21">
+        <v>253.71990000000002</v>
+      </c>
+      <c r="J13" s="21">
+        <v>257.39699999999999</v>
+      </c>
+      <c r="K13" s="21">
+        <v>261.07409999999993</v>
+      </c>
+      <c r="L13" s="21">
+        <v>264.75119999999998</v>
+      </c>
+      <c r="M13" s="21">
+        <v>268.42829999999998</v>
+      </c>
+      <c r="N13" s="21">
+        <v>272.10539999999997</v>
+      </c>
+      <c r="O13" s="21">
+        <v>275.78249999999997</v>
+      </c>
+      <c r="P13" s="21">
+        <v>279.45959999999997</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>283.13669999999996</v>
+      </c>
+      <c r="R13" s="21">
+        <v>286.81380000000001</v>
+      </c>
+      <c r="S13" s="21">
+        <v>290.49090000000001</v>
+      </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B14" s="2">
+        <v>540</v>
+      </c>
+      <c r="C14" s="21">
+        <v>245.28420000000003</v>
+      </c>
+      <c r="D14" s="21">
+        <v>249.17760000000001</v>
+      </c>
+      <c r="E14" s="21">
+        <v>253.071</v>
+      </c>
+      <c r="F14" s="21">
+        <v>256.96440000000001</v>
+      </c>
+      <c r="G14" s="21">
+        <v>260.8578</v>
+      </c>
+      <c r="H14" s="21">
+        <v>264.75120000000004</v>
+      </c>
+      <c r="I14" s="21">
+        <v>268.64460000000003</v>
+      </c>
+      <c r="J14" s="21">
+        <v>272.53800000000001</v>
+      </c>
+      <c r="K14" s="21">
+        <v>276.4314</v>
+      </c>
+      <c r="L14" s="21">
+        <v>280.32479999999998</v>
+      </c>
+      <c r="M14" s="21">
+        <v>284.21819999999997</v>
+      </c>
+      <c r="N14" s="21">
+        <v>288.11160000000001</v>
+      </c>
+      <c r="O14" s="21">
+        <v>292.005</v>
+      </c>
+      <c r="P14" s="21">
+        <v>295.89839999999998</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>299.79179999999997</v>
+      </c>
+      <c r="R14" s="21">
+        <v>303.68519999999995</v>
+      </c>
+      <c r="S14" s="21">
+        <v>307.57860000000005</v>
+      </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B15" s="2">
+        <v>570</v>
+      </c>
+      <c r="C15" s="21">
+        <v>258.91110000000003</v>
+      </c>
+      <c r="D15" s="21">
+        <v>263.02080000000001</v>
+      </c>
+      <c r="E15" s="21">
+        <v>267.13050000000004</v>
+      </c>
+      <c r="F15" s="21">
+        <v>271.24020000000002</v>
+      </c>
+      <c r="G15" s="21">
+        <v>275.34990000000005</v>
+      </c>
+      <c r="H15" s="21">
+        <v>279.45960000000002</v>
+      </c>
+      <c r="I15" s="21">
+        <v>283.56930000000006</v>
+      </c>
+      <c r="J15" s="21">
+        <v>287.67900000000003</v>
+      </c>
+      <c r="K15" s="21">
+        <v>291.78870000000001</v>
+      </c>
+      <c r="L15" s="21">
+        <v>295.89839999999998</v>
+      </c>
+      <c r="M15" s="21">
+        <v>300.00810000000001</v>
+      </c>
+      <c r="N15" s="21">
+        <v>304.11779999999999</v>
+      </c>
+      <c r="O15" s="21">
+        <v>308.22750000000002</v>
+      </c>
+      <c r="P15" s="21">
+        <v>312.3372</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>316.44690000000003</v>
+      </c>
+      <c r="R15" s="21">
+        <v>320.5566</v>
+      </c>
+      <c r="S15" s="21">
+        <v>324.66629999999998</v>
+      </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B16" s="2">
+        <v>600</v>
+      </c>
+      <c r="C16" s="21">
+        <v>272.53799999999995</v>
+      </c>
+      <c r="D16" s="21">
+        <v>276.86399999999998</v>
+      </c>
+      <c r="E16" s="21">
+        <v>281.19</v>
+      </c>
+      <c r="F16" s="21">
+        <v>285.51600000000002</v>
+      </c>
+      <c r="G16" s="21">
+        <v>289.84200000000004</v>
+      </c>
+      <c r="H16" s="21">
+        <v>294.16800000000001</v>
+      </c>
+      <c r="I16" s="21">
+        <v>298.49400000000003</v>
+      </c>
+      <c r="J16" s="21">
+        <v>302.82000000000005</v>
+      </c>
+      <c r="K16" s="21">
+        <v>307.14599999999996</v>
+      </c>
+      <c r="L16" s="21">
+        <v>311.47199999999998</v>
+      </c>
+      <c r="M16" s="21">
+        <v>315.798</v>
+      </c>
+      <c r="N16" s="21">
+        <v>320.12399999999997</v>
+      </c>
+      <c r="O16" s="21">
+        <v>324.45</v>
+      </c>
+      <c r="P16" s="21">
+        <v>328.77600000000001</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>333.10200000000003</v>
+      </c>
+      <c r="R16" s="21">
+        <v>337.428</v>
+      </c>
+      <c r="S16" s="21">
+        <v>341.75399999999996</v>
+      </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <v>630</v>
+      </c>
+      <c r="C17" s="21">
+        <v>286.16489999999999</v>
+      </c>
+      <c r="D17" s="21">
+        <v>290.7072</v>
+      </c>
+      <c r="E17" s="21">
+        <v>295.24950000000001</v>
+      </c>
+      <c r="F17" s="21">
+        <v>299.79180000000002</v>
+      </c>
+      <c r="G17" s="21">
+        <v>304.33409999999998</v>
+      </c>
+      <c r="H17" s="21">
+        <v>308.87640000000005</v>
+      </c>
+      <c r="I17" s="21">
+        <v>313.41870000000006</v>
+      </c>
+      <c r="J17" s="21">
+        <v>317.96100000000001</v>
+      </c>
+      <c r="K17" s="21">
+        <v>322.50329999999997</v>
+      </c>
+      <c r="L17" s="21">
+        <v>327.04559999999998</v>
+      </c>
+      <c r="M17" s="21">
+        <v>331.58789999999993</v>
+      </c>
+      <c r="N17" s="21">
+        <v>336.1302</v>
+      </c>
+      <c r="O17" s="21">
+        <v>340.67250000000001</v>
+      </c>
+      <c r="P17" s="21">
+        <v>345.21479999999997</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>349.75709999999998</v>
+      </c>
+      <c r="R17" s="21">
+        <v>354.29939999999999</v>
+      </c>
+      <c r="S17" s="21">
+        <v>358.8417</v>
+      </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B18" s="2">
+        <v>660</v>
+      </c>
+      <c r="C18" s="21">
+        <v>299.79179999999997</v>
+      </c>
+      <c r="D18" s="21">
+        <v>304.55040000000002</v>
+      </c>
+      <c r="E18" s="21">
+        <v>309.30899999999997</v>
+      </c>
+      <c r="F18" s="21">
+        <v>314.06760000000003</v>
+      </c>
+      <c r="G18" s="21">
+        <v>318.82620000000003</v>
+      </c>
+      <c r="H18" s="21">
+        <v>323.58480000000003</v>
+      </c>
+      <c r="I18" s="21">
+        <v>328.34340000000003</v>
+      </c>
+      <c r="J18" s="21">
+        <v>333.10200000000003</v>
+      </c>
+      <c r="K18" s="21">
+        <v>337.86059999999992</v>
+      </c>
+      <c r="L18" s="21">
+        <v>342.61919999999998</v>
+      </c>
+      <c r="M18" s="21">
+        <v>347.37779999999998</v>
+      </c>
+      <c r="N18" s="21">
+        <v>352.13639999999998</v>
+      </c>
+      <c r="O18" s="21">
+        <v>356.89499999999998</v>
+      </c>
+      <c r="P18" s="21">
+        <v>361.65359999999998</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>366.41219999999998</v>
+      </c>
+      <c r="R18" s="21">
+        <v>371.17079999999999</v>
+      </c>
+      <c r="S18" s="21">
+        <v>375.92939999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B19" s="2">
+        <v>690</v>
+      </c>
+      <c r="C19" s="21">
+        <v>313.4187</v>
+      </c>
+      <c r="D19" s="21">
+        <v>318.39360000000005</v>
+      </c>
+      <c r="E19" s="21">
+        <v>323.36849999999998</v>
+      </c>
+      <c r="F19" s="21">
+        <v>328.34339999999997</v>
+      </c>
+      <c r="G19" s="21">
+        <v>333.31830000000002</v>
+      </c>
+      <c r="H19" s="21">
+        <v>338.29320000000001</v>
+      </c>
+      <c r="I19" s="21">
+        <v>343.26810000000006</v>
+      </c>
+      <c r="J19" s="21">
+        <v>348.24300000000005</v>
+      </c>
+      <c r="K19" s="21">
+        <v>353.21789999999999</v>
+      </c>
+      <c r="L19" s="21">
+        <v>358.19279999999998</v>
+      </c>
+      <c r="M19" s="21">
+        <v>363.16769999999997</v>
+      </c>
+      <c r="N19" s="21">
+        <v>368.14259999999996</v>
+      </c>
+      <c r="O19" s="21">
+        <v>373.11750000000001</v>
+      </c>
+      <c r="P19" s="21">
+        <v>378.0924</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>383.06729999999999</v>
+      </c>
+      <c r="R19" s="21">
+        <v>388.04219999999998</v>
+      </c>
+      <c r="S19" s="21">
+        <v>393.01709999999997</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:S19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5733,8 +8494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40285E56-8A2C-4564-8575-7360840FD5FD}">
   <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="86" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A16" zoomScale="86" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5846,56 +8607,56 @@
       <c r="B6" s="2">
         <v>270</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="21">
         <f t="dataTable" ref="C6:S19" dt2D="1" dtr="1" r1="C3" r2="B3"/>
         <v>35.559000000000005</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="21">
         <v>44.448749999999997</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="21">
         <v>53.338499999999996</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="21">
         <v>62.22825000000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="21">
         <v>71.118000000000009</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="21">
         <v>80.007750000000001</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="21">
         <v>88.897499999999994</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="21">
         <v>97.78725</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="21">
         <v>106.67699999999999</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="21">
         <v>115.56675</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="21">
         <v>124.45650000000002</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="21">
         <v>133.34625</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="21">
         <v>142.23600000000002</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="21">
         <v>151.12575000000001</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="21">
         <v>160.0155</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="21">
         <v>168.90525</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="21">
         <v>177.79499999999999</v>
       </c>
     </row>
@@ -5903,55 +8664,55 @@
       <c r="B7" s="2">
         <v>280</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="21">
         <v>36.876000000000005</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="21">
         <v>46.094999999999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="21">
         <v>55.314</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="21">
         <v>64.533000000000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="21">
         <v>73.75200000000001</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="21">
         <v>82.971000000000004</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="21">
         <v>92.19</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="21">
         <v>101.40900000000001</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="21">
         <v>110.628</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="21">
         <v>119.84699999999999</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="21">
         <v>129.066</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="21">
         <v>138.285</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="21">
         <v>147.50400000000002</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="21">
         <v>156.72300000000001</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="21">
         <v>165.94200000000001</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="21">
         <v>175.161</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="21">
         <v>184.38</v>
       </c>
     </row>
@@ -5959,55 +8720,55 @@
       <c r="B8" s="2">
         <v>290</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="21">
         <v>38.192999999999998</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="21">
         <v>47.741250000000001</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="21">
         <v>57.289499999999997</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="21">
         <v>66.83775</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="21">
         <v>76.385999999999996</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="21">
         <v>85.934249999999992</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="21">
         <v>95.482500000000002</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="21">
         <v>105.03075</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="21">
         <v>114.57899999999999</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="21">
         <v>124.12725</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="21">
         <v>133.6755</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="21">
         <v>143.22375</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="21">
         <v>152.77199999999999</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="21">
         <v>162.32025000000002</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="21">
         <v>171.86849999999998</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="21">
         <v>181.41675000000001</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="21">
         <v>190.965</v>
       </c>
     </row>
@@ -6015,55 +8776,55 @@
       <c r="B9" s="2">
         <v>300</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="21">
         <v>39.51</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="21">
         <v>49.387500000000003</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="21">
         <v>59.265000000000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="21">
         <v>69.142500000000013</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="21">
         <v>79.02</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="21">
         <v>88.897499999999994</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="21">
         <v>98.775000000000006</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="21">
         <v>108.6525</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="21">
         <v>118.53</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="21">
         <v>128.4075</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="21">
         <v>138.28500000000003</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="21">
         <v>148.16249999999999</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="21">
         <v>158.04</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="21">
         <v>167.91750000000002</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="21">
         <v>177.79499999999999</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="21">
         <v>187.67249999999999</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="21">
         <v>197.55</v>
       </c>
     </row>
@@ -6071,55 +8832,55 @@
       <c r="B10" s="2">
         <v>310</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="21">
         <v>40.826999999999998</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="21">
         <v>51.033749999999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="21">
         <v>61.24049999999999</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="21">
         <v>71.447250000000011</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="21">
         <v>81.653999999999996</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="21">
         <v>91.860749999999996</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="21">
         <v>102.0675</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="21">
         <v>112.27425000000001</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="21">
         <v>122.48099999999998</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="21">
         <v>132.68775000000002</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="21">
         <v>142.89450000000002</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="21">
         <v>153.10124999999999</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="21">
         <v>163.30799999999999</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="21">
         <v>173.51475000000002</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="21">
         <v>183.72149999999999</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="21">
         <v>193.92824999999999</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="21">
         <v>204.13499999999999</v>
       </c>
     </row>
@@ -6127,55 +8888,55 @@
       <c r="B11" s="2">
         <v>320</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="21">
         <v>42.144000000000005</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="21">
         <v>52.68</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="21">
         <v>63.215999999999994</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="21">
         <v>73.75200000000001</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="21">
         <v>84.288000000000011</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="21">
         <v>94.823999999999984</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="21">
         <v>105.36</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="21">
         <v>115.89600000000002</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="21">
         <v>126.43199999999999</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="21">
         <v>136.96800000000002</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="21">
         <v>147.50400000000002</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="21">
         <v>158.04</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="21">
         <v>168.57600000000002</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="21">
         <v>179.11200000000002</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="21">
         <v>189.64799999999997</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="21">
         <v>200.184</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="21">
         <v>210.72</v>
       </c>
     </row>
@@ -6183,55 +8944,55 @@
       <c r="B12" s="2">
         <v>330</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="21">
         <v>43.461000000000006</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="21">
         <v>54.326250000000002</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="21">
         <v>65.191500000000005</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="21">
         <v>76.056750000000008</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="21">
         <v>86.922000000000011</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="21">
         <v>97.78725</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="21">
         <v>108.6525</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="21">
         <v>119.51774999999999</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="21">
         <v>130.38300000000001</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="21">
         <v>141.24824999999998</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="21">
         <v>152.11350000000002</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="21">
         <v>162.97874999999999</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="21">
         <v>173.84400000000002</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="21">
         <v>184.70925</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q12" s="21">
         <v>195.5745</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="21">
         <v>206.43975</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="21">
         <v>217.30500000000001</v>
       </c>
     </row>
@@ -6239,55 +9000,55 @@
       <c r="B13" s="2">
         <v>340</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="21">
         <v>44.777999999999999</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="21">
         <v>55.972499999999997</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="21">
         <v>67.167000000000002</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="21">
         <v>78.361500000000007</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="21">
         <v>89.555999999999997</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="21">
         <v>100.75049999999999</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="21">
         <v>111.94499999999999</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="21">
         <v>123.1395</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="21">
         <v>134.334</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="21">
         <v>145.52850000000001</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="21">
         <v>156.72300000000001</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="21">
         <v>167.91749999999999</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="21">
         <v>179.11199999999999</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="21">
         <v>190.3065</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="21">
         <v>201.50099999999998</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="21">
         <v>212.69549999999998</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="21">
         <v>223.89</v>
       </c>
     </row>
@@ -6295,55 +9056,55 @@
       <c r="B14" s="2">
         <v>350</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="21">
         <v>46.094999999999999</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="21">
         <v>57.618749999999999</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="21">
         <v>69.142499999999998</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="21">
         <v>80.666250000000005</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="21">
         <v>92.19</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="21">
         <v>103.71375</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="21">
         <v>115.2375</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="21">
         <v>126.76125</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="21">
         <v>138.285</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="21">
         <v>149.80875</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="21">
         <v>161.33250000000001</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="21">
         <v>172.85624999999999</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="21">
         <v>184.38</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="21">
         <v>195.90375000000003</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="21">
         <v>207.42750000000001</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="21">
         <v>218.95124999999999</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="21">
         <v>230.47499999999999</v>
       </c>
     </row>
@@ -6351,55 +9112,55 @@
       <c r="B15" s="2">
         <v>360</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="21">
         <v>47.411999999999999</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="21">
         <v>59.265000000000001</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="21">
         <v>71.117999999999995</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="21">
         <v>82.971000000000004</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="21">
         <v>94.823999999999998</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="21">
         <v>106.67699999999999</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="21">
         <v>118.53</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="21">
         <v>130.38300000000001</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="21">
         <v>142.23599999999999</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="21">
         <v>154.08900000000003</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="21">
         <v>165.94200000000001</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="21">
         <v>177.79499999999999</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="21">
         <v>189.648</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="21">
         <v>201.501</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q15" s="21">
         <v>213.35399999999998</v>
       </c>
-      <c r="R15" s="1">
+      <c r="R15" s="21">
         <v>225.20700000000002</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="21">
         <v>237.06</v>
       </c>
     </row>
@@ -6407,55 +9168,55 @@
       <c r="B16" s="2">
         <v>370</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="21">
         <v>48.728999999999999</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="21">
         <v>60.911250000000003</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="21">
         <v>73.093499999999992</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="21">
         <v>85.275750000000002</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="21">
         <v>97.457999999999998</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="21">
         <v>109.64024999999999</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="21">
         <v>121.82250000000001</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="21">
         <v>134.00475</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="21">
         <v>146.18699999999998</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="21">
         <v>158.36924999999999</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="21">
         <v>170.5515</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="21">
         <v>182.73374999999999</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="21">
         <v>194.916</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="21">
         <v>207.09825000000001</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q16" s="21">
         <v>219.28049999999999</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16" s="21">
         <v>231.46275</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="21">
         <v>243.64500000000001</v>
       </c>
     </row>
@@ -6463,55 +9224,55 @@
       <c r="B17" s="2">
         <v>380</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="21">
         <v>50.046000000000006</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="21">
         <v>62.557499999999997</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="21">
         <v>75.069000000000003</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="21">
         <v>87.580500000000001</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="21">
         <v>100.09200000000001</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="21">
         <v>112.60349999999998</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="21">
         <v>125.11499999999999</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="21">
         <v>137.62649999999999</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="21">
         <v>150.13800000000001</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="21">
         <v>162.64949999999999</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="21">
         <v>175.161</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="21">
         <v>187.67249999999999</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="21">
         <v>200.18400000000003</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="21">
         <v>212.69550000000004</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q17" s="21">
         <v>225.20699999999997</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17" s="21">
         <v>237.71850000000001</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" s="21">
         <v>250.23</v>
       </c>
     </row>
@@ -6519,55 +9280,55 @@
       <c r="B18" s="2">
         <v>390</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="21">
         <v>51.363</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="21">
         <v>64.203749999999999</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="21">
         <v>77.044499999999999</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="21">
         <v>89.885250000000013</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="21">
         <v>102.726</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="21">
         <v>115.56675</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="21">
         <v>128.4075</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="21">
         <v>141.24824999999998</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="21">
         <v>154.089</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="21">
         <v>166.92975000000001</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="21">
         <v>179.77050000000003</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="21">
         <v>192.61125000000001</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="21">
         <v>205.452</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P18" s="21">
         <v>218.29275000000004</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="21">
         <v>231.1335</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R18" s="21">
         <v>243.97424999999998</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" s="21">
         <v>256.815</v>
       </c>
     </row>
@@ -6575,55 +9336,55 @@
       <c r="B19" s="2">
         <v>400</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="21">
         <v>52.68</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="21">
         <v>65.849999999999994</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="21">
         <v>79.02</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="21">
         <v>92.190000000000012</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="21">
         <v>105.36</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="21">
         <v>118.53</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="21">
         <v>131.69999999999999</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="21">
         <v>144.87</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="21">
         <v>158.04</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="21">
         <v>171.21</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="21">
         <v>184.38000000000002</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="21">
         <v>197.55</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="21">
         <v>210.72</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19" s="21">
         <v>223.89</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="21">
         <v>237.06</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="21">
         <v>250.23</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" s="21">
         <v>263.39999999999998</v>
       </c>
     </row>
@@ -6646,6 +9407,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED077DFD7547DE40BB19C407130BA958" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="30b98e02899bc55dc199837b6108a876">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="146f35c0-5549-4b11-9385-b5bad1d7a6e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8899f713b441a45dc39a6408faeb9f10" ns3:_="">
     <xsd:import namespace="146f35c0-5549-4b11-9385-b5bad1d7a6e6"/>
@@ -6823,22 +9599,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0D16BC9-63C7-4ECC-819E-4E697176BB59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BB1E92-878A-4494-BE21-999963AA96A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C08BEF9B-E79F-4EED-9FBF-FF73572E04B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6854,21 +9632,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BB1E92-878A-4494-BE21-999963AA96A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0D16BC9-63C7-4ECC-819E-4E697176BB59}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>